<commit_message>
Admin company view m. edit & delete done
</commit_message>
<xml_diff>
--- a/Diagrammer/Burndown for WHAT.xlsx
+++ b/Diagrammer/Burndown for WHAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3-sem.-eksamen-SWD\Diagrammer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3.SemesterSWD-Eksamen.Final\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CABE830-D5CF-45AF-A4F6-C338AA2A0D00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32351A04-82A8-492D-A6E7-B7B5BC452852}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
+    <workbookView xWindow="7905" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Est.</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Resterende min</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -271,6 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1427,16 +1431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1761,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748780FD-D025-4A00-ABEB-C79BF8E25DEA}">
-  <dimension ref="B3:O31"/>
+  <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1778,15 @@
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1795,9 +1807,6 @@
         <v>1</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="J3" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>30</v>
       </c>
@@ -1807,10 +1816,16 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1840,8 +1855,14 @@
       <c r="L4" s="9">
         <v>1530</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1871,8 +1892,15 @@
         <f>SUM(L4-C4)</f>
         <v>1440</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <f>SUM(P4-630)</f>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1902,8 +1930,15 @@
         <f>SUM(L5-(C5+C6))</f>
         <v>1200</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f>SUM(P4/3)</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1927,8 +1962,15 @@
         <f>SUM(L6-(C7+C8+C9))</f>
         <v>810</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <f>SUM(P6-630)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1953,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1975,7 +2017,7 @@
       </c>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +2039,7 @@
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -2011,7 +2053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -2025,7 +2067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2039,7 +2081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -2053,7 +2095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -2064,7 +2106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Task network 1 og 2 never more
</commit_message>
<xml_diff>
--- a/Diagrammer/Burndown for WHAT.xlsx
+++ b/Diagrammer/Burndown for WHAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3.SemesterSWD-Eksamen.Final\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32351A04-82A8-492D-A6E7-B7B5BC452852}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AAFA95-0F08-4B0C-95B5-A6877AF9FAD7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
+    <workbookView xWindow="8835" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1765,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748780FD-D025-4A00-ABEB-C79BF8E25DEA}">
-  <dimension ref="B2:Q31"/>
+  <dimension ref="B2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,31 +2223,31 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
+    <row r="35" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C35" s="10">
         <f>SUM(C4:C27)/60</f>
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="36" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38">
         <f>SUM(62*60)-(C4+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14)</f>
         <v>2370</v>
       </c>
-      <c r="C31">
-        <f>SUM(B31/60)</f>
+      <c r="C38">
+        <f>SUM(B38/60)</f>
         <v>39.5</v>
       </c>
     </row>

</xml_diff>